<commit_message>
2022-04-05 : 기능구현 약 80% 수행
</commit_message>
<xml_diff>
--- a/messanger_명세서_real.xlsx
+++ b/messanger_명세서_real.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2022\project\messger_back_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5758B369-79A9-4C65-8E47-77DF03CFE5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66E1E57-E74D-4B28-AB37-5034574D2218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F76E1A7-2D25-49C5-8186-B5B55EB180C4}"/>
   </bookViews>
@@ -34,6 +34,153 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={FA9D0A99-DE01-4D24-A7AF-D469D4B5DE7F}</author>
+    <author>tc={BA602F9A-EBE0-40BB-AAE8-62BDBE591E4F}</author>
+    <author>tc={53DA806B-6C43-4937-A735-F7A7E1605AD5}</author>
+    <author>tc={94E65638-B2C8-404C-9DAF-2381931F9E27}</author>
+    <author>tc={1CC1C6EB-6096-4B35-8C20-75AE8FDF947D}</author>
+    <author>tc={1F9831E2-3FC7-42B0-9139-25B1ADBEF89C}</author>
+    <author>tc={C2A0F362-777D-4761-9AF7-9837E41B1C09}</author>
+    <author>tc={94CEBC5F-9545-4AC7-A477-40B1429538DB}</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{FA9D0A99-DE01-4D24-A7AF-D469D4B5DE7F}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    {
+    "userId": 6,
+    "id": "test6",
+    "pwd": "$2a$10$SBoArhF40sgFsjAO2It/7e2zW/66n.xeIhA4vAap1tfL7dsReb0qi",
+    "name": null,
+    "phone": null,
+    "email": null,
+    "role": "ROLE_USER"
+}</t>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="1" shapeId="0" xr:uid="{BA602F9A-EBE0-40BB-AAE8-62BDBE591E4F}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    {
+    "groupMemberList": [
+        {
+            "groupId": 1,
+            "name": "test2"
+        },
+        {
+            "groupId": 1,
+            "name": "test3"
+        },
+        {
+            "groupId": 2,
+            "name": "test4"
+        },
+        {
+            "groupId": 2,
+            "name": "test5"
+        }
+    ],
+    "groupName": [
+        {
+            "groupName": "we are tester!",
+            "groupId": 1
+        },
+        {
+            "groupName": "꺼져라!",
+            "groupId": 2
+        }
+    ],
+    "groupCount": 2,
+    "userId": 1
+}</t>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="2" shapeId="0" xr:uid="{53DA806B-6C43-4937-A735-F7A7E1605AD5}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    {
+    "groupName": "we are tester!",
+    "groupId": 1
+}</t>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="3" shapeId="0" xr:uid="{94E65638-B2C8-404C-9DAF-2381931F9E27}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    {
+        "promiseId": 1,
+        "promiseName": "test promise",
+        "promiseInfo": "this is test!",
+        "promiseDate": null,
+        "location": null
+    },
+    {
+        "promiseId": 3,
+        "promiseName": "test222",
+        "promiseInfo": "this is test promise",
+        "promiseDate": null,
+        "location": null
+    }</t>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="4" shapeId="0" xr:uid="{1CC1C6EB-6096-4B35-8C20-75AE8FDF947D}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    {
+    "promiseId": 1,
+    "promiseInfo": "this is test!",
+    "groupId": 1,
+    "promiseName": "test promise"
+}</t>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="5" shapeId="0" xr:uid="{1F9831E2-3FC7-42B0-9139-25B1ADBEF89C}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    1</t>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="6" shapeId="0" xr:uid="{C2A0F362-777D-4761-9AF7-9837E41B1C09}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    {
+    "userId": 1
+}</t>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="7" shapeId="0" xr:uid="{94CEBC5F-9545-4AC7-A477-40B1429538DB}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    {
+    "groupId": 3,
+    "successResult": 1,
+    "userId": 1
+}</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
@@ -337,7 +484,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,8 +514,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +543,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +619,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -479,6 +638,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -488,8 +659,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,23 +677,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,6 +710,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="hj" id="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" userId="hj" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -830,12 +1013,107 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E3" dT="2022-04-02T06:53:44.37" personId="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" id="{FA9D0A99-DE01-4D24-A7AF-D469D4B5DE7F}">
+    <text>{
+    "userId": 6,
+    "id": "test6",
+    "pwd": "$2a$10$SBoArhF40sgFsjAO2It/7e2zW/66n.xeIhA4vAap1tfL7dsReb0qi",
+    "name": null,
+    "phone": null,
+    "email": null,
+    "role": "ROLE_USER"
+}</text>
+  </threadedComment>
+  <threadedComment ref="E5" dT="2022-04-02T06:56:48.00" personId="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" id="{BA602F9A-EBE0-40BB-AAE8-62BDBE591E4F}">
+    <text>{
+    "groupMemberList": [
+        {
+            "groupId": 1,
+            "name": "test2"
+        },
+        {
+            "groupId": 1,
+            "name": "test3"
+        },
+        {
+            "groupId": 2,
+            "name": "test4"
+        },
+        {
+            "groupId": 2,
+            "name": "test5"
+        }
+    ],
+    "groupName": [
+        {
+            "groupName": "we are tester!",
+            "groupId": 1
+        },
+        {
+            "groupName": "꺼져라!",
+            "groupId": 2
+        }
+    ],
+    "groupCount": 2,
+    "userId": 1
+}</text>
+  </threadedComment>
+  <threadedComment ref="E6" dT="2022-04-02T07:03:38.75" personId="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" id="{53DA806B-6C43-4937-A735-F7A7E1605AD5}">
+    <text>{
+    "groupName": "we are tester!",
+    "groupId": 1
+}</text>
+  </threadedComment>
+  <threadedComment ref="E7" dT="2022-04-02T07:19:46.82" personId="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" id="{94E65638-B2C8-404C-9DAF-2381931F9E27}">
+    <text>{
+        "promiseId": 1,
+        "promiseName": "test promise",
+        "promiseInfo": "this is test!",
+        "promiseDate": null,
+        "location": null
+    },
+    {
+        "promiseId": 3,
+        "promiseName": "test222",
+        "promiseInfo": "this is test promise",
+        "promiseDate": null,
+        "location": null
+    }</text>
+  </threadedComment>
+  <threadedComment ref="E8" dT="2022-04-02T07:44:21.87" personId="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" id="{1CC1C6EB-6096-4B35-8C20-75AE8FDF947D}">
+    <text>{
+    "promiseId": 1,
+    "promiseInfo": "this is test!",
+    "groupId": 1,
+    "promiseName": "test promise"
+}</text>
+  </threadedComment>
+  <threadedComment ref="E9" dT="2022-04-02T07:47:00.32" personId="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" id="{1F9831E2-3FC7-42B0-9139-25B1ADBEF89C}">
+    <text>1</text>
+  </threadedComment>
+  <threadedComment ref="E10" dT="2022-04-02T07:47:26.38" personId="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" id="{C2A0F362-777D-4761-9AF7-9837E41B1C09}">
+    <text>{
+    "userId": 1
+}</text>
+  </threadedComment>
+  <threadedComment ref="E11" dT="2022-04-02T07:47:53.99" personId="{5C6F9BD3-657B-4C2D-93A8-70304BFB299B}" id="{94CEBC5F-9545-4AC7-A477-40B1429538DB}">
+    <text>{
+    "groupId": 3,
+    "successResult": 1,
+    "userId": 1
+}</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595E765F-3BB3-4B57-91E9-CC05AADA25C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595E765F-3BB3-4B57-91E9-CC05AADA25C1}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -849,41 +1127,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -898,36 +1176,36 @@
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -942,13 +1220,13 @@
       <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -957,19 +1235,19 @@
       <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" ht="99" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -984,13 +1262,13 @@
       <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1005,13 +1283,13 @@
       <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1026,13 +1304,13 @@
       <c r="E9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1047,13 +1325,13 @@
       <c r="E10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="99" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1068,13 +1346,13 @@
       <c r="E11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:9" ht="363" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1089,13 +1367,13 @@
       <c r="E12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1110,15 +1388,15 @@
       <c r="E13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="8"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1133,12 +1411,12 @@
       <c r="E14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -1296,22 +1574,23 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="F5:I5"/>
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="F11:I11"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="F9:I9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>